<commit_message>
added other tables (output errors)
</commit_message>
<xml_diff>
--- a/movie_summary.xlsx
+++ b/movie_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,31 @@
           <t>Plot</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cast</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Release Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Runtime</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Rating</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,12 +483,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Genre not available</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Dom Cobb and Arthur are "extractors" who perform corporate espionage using experimental dream-sharing technology to infiltrate their targets' subconscious and extract information. Their latest target, Saito, is impressed with Cobb's ability to layer multiple dreams within each other. He offers to hire Cobb for the ostensibly impossible job of implanting an idea into a person's subconscious; performing "inception" on Robert Fischer, the son of Saito's competitor Maurice Fischer, with the idea to dissolve his father's company. In return, Saito promises to clear Cobb's criminal status, allowing him to return home to his children.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Not found</t>
         </is>
       </c>
     </row>
@@ -475,12 +525,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Action, Drama</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>In 1945, the New York City Corleone family don, Vito Corleone, listens to requests during his daughter Connie's wedding to Carlo Rizzi. Vito's youngest son Michael, a Marine and World War II hero who has so far stayed out of the family business, introduces his girlfriend Kay Adams to his family at the reception. Johnny Fontane, a popular singer and Vito's godson, seeks Vito's help in securing a movie role. Vito sends his consigliere Tom Hagen to persuade studio president Jack Woltz to offer Johnny the part. Woltz refuses Hagen's request at first, but soon complies after finding the severed head of his prized stud horse in his bed.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Not found</t>
         </is>
       </c>
     </row>
@@ -492,10 +567,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Genre not available</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t>In the mid-21st century, humanity faces extinction due to dust storms and widespread crop blights. Joseph Cooper, a widowed former NASA test pilot, works as a farmer and raises his children, Murph and Tom, alongside his father-in-law Donald. Living in a post-truth society, Cooper is reprimanded by Murph's teachers for telling her that the Apollo missions were not fabricated. During a dust storm, the two discover that dust patterns in Murph's room, which she first attributes to a ghost, result from a gravitational anomaly, and translate into geographic coordinates. These lead them to a secret NASA facility headed by Professor John Brand, who explains that, 48 years earlier, a wormhole appeared near Saturn, leading to a system in another galaxy with twelve potentially habitable planets located near a black hole named Gargantua. Volunteers of the Lazarus expedition had previously travelled through the wormhole to evaluate the planets, with Miller, Edmunds, and Mann reporting back desirable results.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Not found</t>
         </is>
@@ -509,12 +609,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Genre not available</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>In 1981, a feather lands at a bus stop in Savannah, Georgia, where a man named Forrest Gump recounts his life story to strangers who sit next to him on a bench.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Not found</t>
         </is>
       </c>
     </row>
@@ -526,7 +651,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Sci-Fi</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -534,89 +659,29 @@
           <t>In 2018, 23 days after Thanos erased half of all life in the universe,[a] Carol Danvers rescues Tony Stark and Nebula from deep space. They reunite with the remaining Avengers—Bruce Banner, Steve Rogers, Thor, Natasha Romanoff, and James Rhodes—and Rocket on Earth. Locating Thanos on an uninhabited planet, they plan to use the Infinity Stones to reverse his actions but find that Thanos has destroyed them. Enraged, Thor decapitates Thanos.</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Inception</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Dom Cobb and Arthur are "extractors" who perform corporate espionage using experimental dream-sharing technology to infiltrate their targets' subconscious and extract information. Their latest target, Saito, is impressed with Cobb's ability to layer multiple dreams within each other. He offers to hire Cobb for the ostensibly impossible job of implanting an idea into a person's subconscious; performing "inception" on Robert Fischer, the son of Saito's competitor Maurice Fischer, with the idea to dissolve his father's company. In return, Saito promises to clear Cobb's criminal status, allowing him to return home to his children.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>The Godfather</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>In 1945, the New York City Corleone family don, Vito Corleone, listens to requests during his daughter Connie's wedding to Carlo Rizzi. Vito's youngest son Michael, a Marine and World War II hero who has so far stayed out of the family business, introduces his girlfriend Kay Adams to his family at the reception. Johnny Fontane, a popular singer and Vito's godson, seeks Vito's help in securing a movie role. Vito sends his consigliere Tom Hagen to persuade studio president Jack Woltz to offer Johnny the part. Woltz refuses Hagen's request at first, but soon complies after finding the severed head of his prized stud horse in his bed.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Interstellar</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Forrest Gump</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>In 1981, a feather lands at a bus stop in Savannah, Georgia, where a man named Forrest Gump recounts his life story to strangers who sit next to him on a bench.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Avengers: Endgame</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>In 2018, 23 days after Thanos erased half of all life in the universe,[a] Carol Danvers rescues Tony Stark and Nebula from deep space. They reunite with the remaining Avengers—Bruce Banner, Steve Rogers, Thor, Natasha Romanoff, and James Rhodes—and Rocket on Earth. Locating Thanos on an uninhabited planet, they plan to use the Infinity Stones to reverse his actions but find that Thanos has destroyed them. Enraged, Thor decapitates Thanos.</t>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Not found</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
plot, director, cast, release date and runtime of everymovie can be found using web scrapping, rating and genre of few movies is left.
</commit_message>
<xml_diff>
--- a/movie_summary.xlsx
+++ b/movie_summary.xlsx
@@ -488,27 +488,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dom Cobb and Arthur are "extractors" who perform corporate espionage using experimental dream-sharing technology to infiltrate their targets' subconscious and extract information. Their latest target, Saito, is impressed with Cobb's ability to layer multiple dreams within each other. He offers to hire Cobb for the ostensibly impossible job of implanting an idea into a person's subconscious; performing "inception" on Robert Fischer, the son of Saito's competitor Maurice Fischer, with the idea to dissolve his father's company. In return, Saito promises to clear Cobb's criminal status, allowing him to return home to his children.</t>
+          <t>Dom Cobb and Arthur are "extractors" who performcorporate espionageusing experimental dream-sharing technology to infiltrate their targets'subconsciousand extract information. Their latest target, Saito, is impressed with Cobb's ability tolayer multiple dreams within each other. He offers to hire Cobb for the ostensibly impossible job of implanting an idea into a person's subconscious; performing "inception" on Robert Fischer, the son of Saito's competitor Maurice Fischer, with the idea to dissolve his father's company. In return, Saito promises to clear Cobb's criminal status, allowing him to return home to his children.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Christopher Nolan</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Leonardo DiCaprio, Leonardo DiCaprio, Ken Watanabe, Ken Watanabe, Joseph Gordon-Levitt, Joseph Gordon-Levitt, Marion Cotillard, Marion Cotillard, Elliot Page[a], Elliot Page, [a], Tom Hardy, Tom Hardy, Cillian Murphy, Cillian Murphy, Tom Berenger, Tom Berenger, Michael Caine, Michael Caine</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>July 8, 2010(2010-07-08)(Odeon Leicester Square)July 16, 2010(2010-07-16)(United States and United Kingdom)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>148 minutes[1]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -530,27 +530,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>In 1945, the New York City Corleone family don, Vito Corleone, listens to requests during his daughter Connie's wedding to Carlo Rizzi. Vito's youngest son Michael, a Marine and World War II hero who has so far stayed out of the family business, introduces his girlfriend Kay Adams to his family at the reception. Johnny Fontane, a popular singer and Vito's godson, seeks Vito's help in securing a movie role. Vito sends his consigliere Tom Hagen to persuade studio president Jack Woltz to offer Johnny the part. Woltz refuses Hagen's request at first, but soon complies after finding the severed head of his prized stud horse in his bed.</t>
+          <t>In 1945, theNew York CityCorleone familydon,Vito Corleone, listens to requests during his daughterConnie's wedding toCarlo Rizzi. Vito's youngest sonMichael, aMarineandWorld War IIhero who has so far stayed out of the family business, introduces his girlfriendKay Adamsto his family at the reception. Johnny Fontane, a popular singer and Vito'sgodson, seeks Vito's help in securing a movie role. Vito sends hisconsigliereTom Hagento persuade studio president Jack Woltz to offer Johnny the part. Woltz refuses Hagen's request at first, but soon complies after finding the severed head of his prized stud horse in his bed.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Francis Ford Coppola</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Marlon Brando, Marlon Brando, Al Pacino, Al Pacino, James Caan, James Caan, Richard Castellano, Richard Castellano, Robert Duvall, Robert Duvall, Sterling Hayden, Sterling Hayden, John Marley, John Marley, Richard Conte, Richard Conte, Diane Keaton, Diane Keaton</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>March 14, 1972(1972-03-14)(Loew's State Theatre)March 24, 1972(1972-03-24)(United States)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>175 minutes[1]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -572,27 +572,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>In the mid-21st century, humanity faces extinction due to dust storms and widespread crop blights. Joseph Cooper, a widowed former NASA test pilot, works as a farmer and raises his children, Murph and Tom, alongside his father-in-law Donald. Living in a post-truth society, Cooper is reprimanded by Murph's teachers for telling her that the Apollo missions were not fabricated. During a dust storm, the two discover that dust patterns in Murph's room, which she first attributes to a ghost, result from a gravitational anomaly, and translate into geographic coordinates. These lead them to a secret NASA facility headed by Professor John Brand, who explains that, 48 years earlier, a wormhole appeared near Saturn, leading to a system in another galaxy with twelve potentially habitable planets located near a black hole named Gargantua. Volunteers of the Lazarus expedition had previously travelled through the wormhole to evaluate the planets, with Miller, Edmunds, and Mann reporting back desirable results.</t>
+          <t>In the mid-21st century, humanity facesextinctiondue todust stormsand widespread cropblights. Joseph Cooper, a widowed formerNASAtest pilot, works as a farmer and raises his children, Murph and Tom, alongside his father-in-law Donald. Living in apost-truth society, Cooper is reprimanded by Murph's teachers for telling her that theApollo missionswere not fabricated. During a dust storm, the two discover that dust patterns in Murph's room, which she first attributes to aghost, result from a gravitational anomaly, and translate intogeographic coordinates. These lead them to a secret NASA facility headed by Professor John Brand, who explains that, 48 years earlier, awormholeappeared nearSaturn, leading to a system in anothergalaxywith twelve potentially habitable planets located near ablack holenamed Gargantua. Volunteers of theLazarusexpedition had previously travelled through the wormhole to evaluate the planets, with Miller, Edmunds, and Mann reporting back desirable results.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Christopher Nolan</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Matthew McConaughey, Matthew McConaughey, Anne Hathaway, Anne Hathaway, Jessica Chastain, Jessica Chastain, Bill Irwin, Bill Irwin, Ellen Burstyn, Ellen Burstyn, Michael Caine, Michael Caine</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>October 26, 2014(2014-10-26)(TCL Chinese Theatre)November 5, 2014(2014-11-05)(United States)November 7, 2014(2014-11-07)(United Kingdom)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>169 minutes[1]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -614,27 +614,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>In 1981, a feather lands at a bus stop in Savannah, Georgia, where a man named Forrest Gump recounts his life story to strangers who sit next to him on a bench.</t>
+          <t>In 1981, a feather lands at a bus stop inSavannah, Georgia, where a man named Forrest Gump recounts his life story to strangers who sit next to him on a bench.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Robert Zemeckis</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Tom Hanks, Tom Hanks, Robin Wright, Robin Wright, Gary Sinise, Gary Sinise, Mykelti Williamson, Mykelti Williamson, Sally Field, Sally Field</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>June 23, 1994(1994-06-23)(Los Angeles)July 6, 1994(1994-07-06)(United States)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>142 minutes</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -656,27 +656,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>In 2018, 23 days after Thanos erased half of all life in the universe,[a] Carol Danvers rescues Tony Stark and Nebula from deep space. They reunite with the remaining Avengers—Bruce Banner, Steve Rogers, Thor, Natasha Romanoff, and James Rhodes—and Rocket on Earth. Locating Thanos on an uninhabited planet, they plan to use the Infinity Stones to reverse his actions but find that Thanos has destroyed them. Enraged, Thor decapitates Thanos.</t>
+          <t>In 2018, 23 days afterThanoserased half of all life in the universe,[a]Carol DanversrescuesTony StarkandNebulafrom deep space. They reunite with the remainingAvengers—Bruce Banner,Steve Rogers,Thor,Natasha Romanoff, andJames Rhodes—andRocketon Earth. Locating Thanos onan uninhabited planet, they plan to use theInfinity Stonesto reverse his actions but find that Thanos has destroyed them. Enraged, Thor decapitates Thanos.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Anthony RussoJoe Russo, Anthony Russo, Joe Russo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Robert Downey Jr., Robert Downey Jr., Chris Evans, Chris Evans, Mark Ruffalo, Mark Ruffalo, Chris Hemsworth, Chris Hemsworth, Scarlett Johansson, Scarlett Johansson, Jeremy Renner, Jeremy Renner, Don Cheadle, Don Cheadle, Paul Rudd, Paul Rudd, Brie Larson, Brie Larson, Karen Gillan, Karen Gillan, Danai Gurira, Danai Gurira, Benedict Wong, Benedict Wong, Jon Favreau, Jon Favreau, Bradley Cooper, Bradley Cooper, Gwyneth Paltrow, Gwyneth Paltrow, Josh Brolin, Josh Brolin</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>April 22, 2019(2019-04-22)(Los Angeles Convention Center)April 26, 2019(2019-04-26)(United States)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>181 minutes[1]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">

</xml_diff>

<commit_message>
rating issue still not fixed.
</commit_message>
<xml_diff>
--- a/movie_summary.xlsx
+++ b/movie_summary.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Genre not available</t>
+          <t>Not found</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Genre not available</t>
+          <t>Not found</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Genre not available</t>
+          <t>Not found</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">

</xml_diff>